<commit_message>
ready for deplyoment on render.com
</commit_message>
<xml_diff>
--- a/shopify_without_livechat.xlsx
+++ b/shopify_without_livechat.xlsx
@@ -1,37 +1,160 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Shopify</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Contact Form</t>
+  </si>
+  <si>
+    <t>Live Chat Solution</t>
+  </si>
+  <si>
+    <t>https://www.luggagefactory.com/</t>
+  </si>
+  <si>
+    <t>https://lazarsluggage.com/</t>
+  </si>
+  <si>
+    <t>https://www.califluggage.com/collections/luggage</t>
+  </si>
+  <si>
+    <t>https://monos.com/</t>
+  </si>
+  <si>
+    <t>https://voyageluggage.com/</t>
+  </si>
+  <si>
+    <t>https://www.califluggage.com/</t>
+  </si>
+  <si>
+    <t>https://www.worldtraveler.com/</t>
+  </si>
+  <si>
+    <t>https://liebers.com/</t>
+  </si>
+  <si>
+    <t>https://shop.tropicfeel.com/collections/backpacks-luggage</t>
+  </si>
+  <si>
+    <t>https://www.lexingtonluggage.com/</t>
+  </si>
+  <si>
+    <t>https://www.muji.us/collections/luggage</t>
+  </si>
+  <si>
+    <t>https://ful.com/</t>
+  </si>
+  <si>
+    <t>Untitled-2_cda00be6-b25a-4f4e-87a8-17254b5ee507_500x@2x.jpg</t>
+  </si>
+  <si>
+    <t>info@lazarsluggage.com</t>
+  </si>
+  <si>
+    <t>caluggage@att.net</t>
+  </si>
+  <si>
+    <t>hello@monos.com</t>
+  </si>
+  <si>
+    <t>example@domain.com</t>
+  </si>
+  <si>
+    <t>1920-Logo_2_200x@2x.jpg</t>
+  </si>
+  <si>
+    <t>EMAILSIG2_180x@2x.jpg</t>
+  </si>
+  <si>
+    <t>online@muji.ca</t>
+  </si>
+  <si>
+    <t>https://www.luggagefactory.com/pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://lazarsluggage.com//pages/contact</t>
+  </si>
+  <si>
+    <t>https://www.califluggage.com/collections/luggage/pages/store-hours</t>
+  </si>
+  <si>
+    <t>https://monos.com//pages/faq</t>
+  </si>
+  <si>
+    <t>https://voyageluggage.com//pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://www.califluggage.com//pages/store-hours</t>
+  </si>
+  <si>
+    <t>https://www.worldtraveler.com//pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://liebers.com//pages/contact</t>
+  </si>
+  <si>
+    <t>https://shop.tropicfeel.com/collections/backpacks-luggage/pages/support</t>
+  </si>
+  <si>
+    <t>https://www.lexingtonluggage.com//pages/store-location-hours</t>
+  </si>
+  <si>
+    <t>https://ful.com//pages/contact-us</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +169,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,89 +491,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Contact Form</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Live Chat Solution</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.califluggage.com/collections/luggage</t>
-        </is>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>caluggage@att.net</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.califluggage.com/collections/luggage/pages/store-hours</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://lazarsluggage.com/</t>
-        </is>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>info@lazarsluggage.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://lazarsluggage.com//pages/contact</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
+    <hyperlink ref="D5" r:id="rId8"/>
+    <hyperlink ref="A6" r:id="rId9"/>
+    <hyperlink ref="D6" r:id="rId10"/>
+    <hyperlink ref="A7" r:id="rId11"/>
+    <hyperlink ref="D7" r:id="rId12"/>
+    <hyperlink ref="A8" r:id="rId13"/>
+    <hyperlink ref="D8" r:id="rId14"/>
+    <hyperlink ref="A9" r:id="rId15"/>
+    <hyperlink ref="D9" r:id="rId16"/>
+    <hyperlink ref="A10" r:id="rId17"/>
+    <hyperlink ref="D10" r:id="rId18"/>
+    <hyperlink ref="A11" r:id="rId19"/>
+    <hyperlink ref="D11" r:id="rId20"/>
+    <hyperlink ref="A12" r:id="rId21"/>
+    <hyperlink ref="A13" r:id="rId22"/>
+    <hyperlink ref="D13" r:id="rId23"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added stream of the table and darkmode
</commit_message>
<xml_diff>
--- a/shopify_without_livechat.xlsx
+++ b/shopify_without_livechat.xlsx
@@ -1,37 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Shopify</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Contact_Form</t>
+  </si>
+  <si>
+    <t>Live_Chat_Solution</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +69,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,89 +385,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Shopify</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Contact Form</t>
-        </is>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Live Chat Solution</t>
-        </is>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.califluggage.com/collections/luggage</t>
-        </is>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>caluggage@att.net</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.califluggage.com/collections/luggage/pages/store-hours</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://lazarsluggage.com/</t>
-        </is>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>info@lazarsluggage.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://lazarsluggage.com//pages/contact</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>